<commit_message>
Add tutorial lessons to qXL doc folder.
Add qQueryRange description and docu.
Add Troubleshooting
</commit_message>
<xml_diff>
--- a/doc/examples/Worksheet-Examples.xlsx
+++ b/doc/examples/Worksheet-Examples.xlsx
@@ -5,22 +5,22 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\DEVnet\Projects\Open sourcing KDB tools\qXL\Slides\Tutorial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev237\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="8340" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="10" r:id="rId1"/>
     <sheet name="qOpen qClose" sheetId="8" r:id="rId2"/>
     <sheet name="qQuery" sheetId="9" r:id="rId3"/>
-    <sheet name="qAtom" sheetId="11" r:id="rId4"/>
-    <sheet name="qList" sheetId="2" r:id="rId5"/>
-    <sheet name="qDict" sheetId="4" r:id="rId6"/>
-    <sheet name="qTable" sheetId="7" r:id="rId7"/>
-    <sheet name="data" sheetId="6" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId9"/>
+    <sheet name="qQueryRange" sheetId="12" r:id="rId4"/>
+    <sheet name="qAtom" sheetId="11" r:id="rId5"/>
+    <sheet name="qList" sheetId="2" r:id="rId6"/>
+    <sheet name="qDict" sheetId="4" r:id="rId7"/>
+    <sheet name="qTable" sheetId="7" r:id="rId8"/>
+    <sheet name="data" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="106">
   <si>
     <t>Result</t>
   </si>
@@ -371,6 +371,69 @@
   </si>
   <si>
     <t>=qQuery(C1,"ungroup 0!select raze raze enlist colB by colA from t2")</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,"1b")</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,"2+2")</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,".z.D")</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,"10* 1 2 3")</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,"func",3,10)</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,"triple:{[p] :3*p}")</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,"triple",40)</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,"getMax",qList(D11:F11,"i"))</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,"t1")</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,t1)</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,"select from t2 where colA=`d")</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,"select from t2 where colA=`c")</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1, "flip last select from t2 where colA=`c")</t>
+  </si>
+  <si>
+    <t>=qQueryRange(C1,"ungroup 0!select raze raze enlist colB by colA from t2")</t>
+  </si>
+  <si>
+    <t>colB</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>sym1</t>
+  </si>
+  <si>
+    <t>sym2</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -660,6 +723,73 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>923927</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152402</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Left-Up Arrow 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6657977" y="342902"/>
+          <a:ext cx="3609973" cy="3086098"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftUpArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2740"/>
+            <a:gd name="adj2" fmla="val 3072"/>
+            <a:gd name="adj3" fmla="val 6257"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1431,7 +1561,7 @@
   <dimension ref="A1:V45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF63" sqref="AF63"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,19 +1716,19 @@
       </c>
       <c r="C11" s="5">
         <f ca="1">_xll.qQuery(C1,"getMax",_xll.qList(D11:F11,"f"))</f>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="D11" s="5">
         <f t="array" ref="D11:F11" ca="1">INT(100*RAND())</f>
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E11" s="5">
         <f ca="1"/>
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="F11">
         <f ca="1"/>
-        <v>46</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -2054,6 +2184,631 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:V45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" hidden="1" customWidth="1"/>
+    <col min="8" max="19" width="0" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f>_xll.qOpen("testConnection","localhost",5001)</f>
+        <v>testConnection</v>
+      </c>
+      <c r="T1" s="42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="5" t="b">
+        <f>_xll.qQueryRange(C1,"1b")</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="5">
+        <f>_xll.qQueryRange(C1,"2+2")</f>
+        <v>4</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="5">
+        <f>_xll.qQueryRange(C1,".z.D")</f>
+        <v>41961</v>
+      </c>
+      <c r="D5" s="6">
+        <f>C5</f>
+        <v>41961</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="5">
+        <f>_xll.qQueryRange(C1,"10 * 1 2 3")</f>
+        <v>10</v>
+      </c>
+      <c r="D6" s="5">
+        <v>20</v>
+      </c>
+      <c r="E6" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="5" t="str">
+        <f>_xll.qQueryRange(C1,"func",3,10)</f>
+        <v>ERR: func</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f>_xll.qQueryRange(C1,"triple:{[p] :3*p}")</f>
+        <v>triple:{[p] :3*p}</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="5">
+        <f>_xll.qQueryRange(C1,"triple",40)</f>
+        <v>120</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="5">
+        <f ca="1">_xll.qQueryRange(C1,"getMax",_xll.qList(D11:F11,"f"))</f>
+        <v>86</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="array" ref="D11:F11" ca="1">INT(100*RAND())</f>
+        <v>40</v>
+      </c>
+      <c r="E11" s="5">
+        <f ca="1"/>
+        <v>22</v>
+      </c>
+      <c r="F11">
+        <f ca="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="9" t="str">
+        <f>_xll.qQueryRange(C1,"t1")</f>
+        <v>colA</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="8">
+        <v>3</v>
+      </c>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="4" t="str">
+        <f>_xll.qQueryRange(C1,T1)</f>
+        <v>ERR: table</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="9" t="str">
+        <f>_xll.qQueryRange(C1,"select from t2 where colA=`d")</f>
+        <v>colA</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="9" t="str">
+        <f>_xll.qQueryRange(C1,"select from t2 where colA=`c")</f>
+        <v>colA</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="9" t="str">
+        <f>_xll.qQueryRange(C1, "flip last select from t2 where colA=`c")</f>
+        <v>colA</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="9" t="str">
+        <f>_xll.qQueryRange(C1,"ungroup 0!select raze raze enlist colB by colA from t2")</f>
+        <v>colA</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="8">
+        <v>1</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="8">
+        <v>2</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="8">
+        <v>3</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="8">
+        <v>1</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="8">
+        <v>2</v>
+      </c>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="8">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:G19"/>
@@ -2191,12 +2946,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2540,7 +3295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L9"/>
@@ -2711,7 +3466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G9"/>
@@ -2881,7 +3636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E5"/>
@@ -2987,19 +3742,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>